<commit_message>
final completed minards map
</commit_message>
<xml_diff>
--- a/nightangle-rose/nightingale-data-1.xlsx
+++ b/nightangle-rose/nightingale-data-1.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9751ff342b8103d3/Documents/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TCD\Semester 2\DataVisualization\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74304AA-824E-480E-974F-8EB76FB356E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{319695F6-E4B8-4708-BD38-2C938BF23956}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{319695F6-E4B8-4708-BD38-2C938BF23956}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>Deaths</t>
   </si>
@@ -191,11 +193,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,676 +513,1120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059C76E7-3BD2-4B3D-B80E-65D861659B83}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8571</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23333</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>28333</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>28722</v>
+      </c>
+      <c r="C5" s="2">
+        <v>150</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>30246</v>
+      </c>
+      <c r="C6" s="2">
+        <v>328.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>30290</v>
+      </c>
+      <c r="C7" s="2">
+        <v>312.2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30643</v>
+      </c>
+      <c r="C8" s="2">
+        <v>197</v>
+      </c>
+      <c r="D8" s="2">
+        <v>51.7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>50.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>29736</v>
+      </c>
+      <c r="C9" s="2">
+        <v>340.6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>115.8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>32779</v>
+      </c>
+      <c r="C10" s="2">
+        <v>631.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>41.7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>32393</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1022.8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>30.7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>30919</v>
+      </c>
+      <c r="C12" s="2">
+        <v>822.8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>16.3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>140.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>30107</v>
+      </c>
+      <c r="C13" s="2">
+        <v>480.3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12.8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>32252</v>
+      </c>
+      <c r="C14" s="2">
+        <v>177.5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E14" s="2">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <v>35473</v>
+      </c>
+      <c r="C15" s="2">
+        <v>171.8</v>
+      </c>
+      <c r="D15" s="2">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
+        <v>38863</v>
+      </c>
+      <c r="C16" s="2">
+        <v>247.6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
+        <v>42647</v>
+      </c>
+      <c r="C17" s="2">
+        <v>107.5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E17" s="2">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2">
+        <v>44614</v>
+      </c>
+      <c r="C18" s="2">
+        <v>129.9</v>
+      </c>
+      <c r="D18" s="2">
+        <v>44.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2">
+        <v>47751</v>
+      </c>
+      <c r="C19" s="2">
+        <v>47.5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2">
+        <v>46852</v>
+      </c>
+      <c r="C20" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D20" s="2">
+        <v>13.6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2">
+        <v>37853</v>
+      </c>
+      <c r="C21" s="2">
+        <v>56.4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="E21" s="2">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43217</v>
+      </c>
+      <c r="C22" s="2">
+        <v>25.3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44212</v>
+      </c>
+      <c r="C23" s="2">
+        <v>11.4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2">
+        <v>43485</v>
+      </c>
+      <c r="C24" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="2">
+        <v>46140</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>9.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839E9DC7-057A-419F-A9D3-2B7967374BE5}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="36" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>8571</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>1.4</v>
       </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>23333</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
         <v>9</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>6.2</v>
       </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>28333</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>11</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>6</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>4.7</v>
       </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>28722</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>359</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
         <v>23</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>150</v>
       </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
         <v>9.6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>30246</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>828</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>30</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>328.5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>0.4</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>11.9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>30290</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>788</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>81</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>70</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>312.2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>32.1</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>27.7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>30643</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>503</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>132</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>128</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>197</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>51.7</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>50.1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>29736</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>844</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>287</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>106</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>340.6</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>115.8</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>42.8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>32779</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>1725</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>114</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>131</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>631.5</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>41.7</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>32393</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>2761</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>83</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>324</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>1022.8</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>30.7</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>30919</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>2120</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>42</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>361</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>822.8</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>16.3</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>140.1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>30107</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>1205</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>32</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>172</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>480.3</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>12.8</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>68.599999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>32252</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>477</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>48</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>57</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>177.5</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>17.899999999999999</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>21.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>35473</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>508</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>49</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>37</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>171.8</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>12.5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>38863</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>802</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>209</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>31</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>247.6</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>64.5</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>9.6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>42647</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>382</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>134</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>33</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>107.5</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>37.700000000000003</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>44614</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>483</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>164</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>25</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>129.9</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>44.1</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>6.7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>47751</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>189</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>276</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>20</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>47.5</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>69.400000000000006</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>46852</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>128</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>53</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>18</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>32.799999999999997</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>13.6</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>37853</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>178</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>33</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>32</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>56.4</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>10.5</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>10.1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>43217</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>91</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>18</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>28</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>25.3</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>5</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>7.8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>44212</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>42</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>2</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>48</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>11.4</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>0.5</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>43485</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>24</v>
       </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
         <v>19</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>6.6</v>
       </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
         <v>5.2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>46140</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>15</v>
       </c>
-      <c r="D26" s="3">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
         <v>35</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>3.9</v>
       </c>
-      <c r="G26" s="3">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
         <v>9.1</v>
       </c>
     </row>

</xml_diff>